<commit_message>
Recomputed Bank M1 for other DR techniques and compiled it
</commit_message>
<xml_diff>
--- a/Experiments/dimensionality_reduction_metrics/results/compiled_results/M1/K-PCA/Bank.xlsx
+++ b/Experiments/dimensionality_reduction_metrics/results/compiled_results/M1/K-PCA/Bank.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,9 +447,65 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.9600122695046023</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0.9518562614462791</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0.9478176730952024</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>5</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.9458168575092269</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>6</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0.9456571933548517</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>7</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0.9455623965112731</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>8</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0.9454888694856882</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
         <v>10</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B9" t="n">
         <v>0.9454018282780285</v>
       </c>
     </row>

</xml_diff>